<commit_message>
excel file open/close bug fix + updated snapshot version for query-repo
</commit_message>
<xml_diff>
--- a/src/main/resources/profile2/Table1.xlsx
+++ b/src/main/resources/profile2/Table1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunny/apps/Intellij-projects/widequery-example-repo/src/main/resources/profile2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjay/intellij/widequery-example-repo/src/main/resources/profile2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C707EE99-42C0-4647-A9A6-0C69E4D8A6EB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C111E442-1E85-6B42-95B2-C6B5984BCF9A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="16940" windowWidth="27640" xWindow="16300" xr2:uid="{B070CAB0-29B0-1E48-B724-2007B49628FA}" yWindow="2700"/>
+    <workbookView activeTab="2" windowHeight="16940" windowWidth="27640" xWindow="16300" xr2:uid="{B070CAB0-29B0-1E48-B724-2007B49628FA}" yWindow="2700"/>
   </bookViews>
   <sheets>
     <sheet name="TableSchema" r:id="rId1" sheetId="1"/>
@@ -389,6 +389,168 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <border diagonalDown="0" diagonalUp="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <border diagonalDown="0" diagonalUp="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <border diagonalDown="0" diagonalUp="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <border diagonalDown="0" diagonalUp="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <border diagonalDown="0" diagonalUp="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <border diagonalDown="0" diagonalUp="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <border diagonalDown="0" diagonalUp="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -409,109 +571,11 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
       <border diagonalDown="0" diagonalUp="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-      <border diagonalDown="0" diagonalUp="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-      <border diagonalDown="0" diagonalUp="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-      <border diagonalDown="0" diagonalUp="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-      <border diagonalDown="0" diagonalUp="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-      <border diagonalDown="0" diagonalUp="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -548,13 +612,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -564,6 +621,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -586,70 +650,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-      <border diagonalDown="0" diagonalUp="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" indent="0" justifyLastLine="0" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-      <border diagonalDown="0" diagonalUp="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -666,34 +666,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Table1" headerRowBorderDxfId="16" headerRowDxfId="12" id="1" mc:Ignorable="xr xr3" name="Table1" ref="B3:C9" tableBorderDxfId="17" totalsRowBorderDxfId="15" totalsRowShown="0" xr:uid="{18445154-F4B3-D547-9CEC-6E41CF4831CF}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" displayName="Table1" headerRowBorderDxfId="16" headerRowDxfId="17" id="1" mc:Ignorable="xr xr3" name="Table1" ref="B3:C9" tableBorderDxfId="15" totalsRowBorderDxfId="14" totalsRowShown="0" xr:uid="{18445154-F4B3-D547-9CEC-6E41CF4831CF}">
   <autoFilter ref="B3:C9" xr:uid="{18445154-F4B3-D547-9CEC-6E41CF4831CF}"/>
   <tableColumns count="2">
-    <tableColumn dataDxfId="14" id="1" name="Column Name" xr3:uid="{5A1F5E39-7036-8D49-AB74-FA0DBA64BFFD}"/>
-    <tableColumn dataDxfId="13" id="2" name="Type" xr3:uid="{33CF3B5F-A7BF-C843-AD10-77B6FFAC8E85}"/>
+    <tableColumn dataDxfId="13" id="1" name="Column Name" xr3:uid="{5A1F5E39-7036-8D49-AB74-FA0DBA64BFFD}"/>
+    <tableColumn dataDxfId="12" id="2" name="Type" xr3:uid="{33CF3B5F-A7BF-C843-AD10-77B6FFAC8E85}"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="1" displayName="Table2" headerRowBorderDxfId="10" headerRowDxfId="0" id="2" mc:Ignorable="xr xr3" name="Table2" ref="B3:H8" tableBorderDxfId="11" totalsRowBorderDxfId="9" totalsRowShown="0" xr:uid="{1D0FFA7F-7DA9-724C-B45B-9B3B656FBCA4}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="9" displayName="Table2" headerRowBorderDxfId="10" headerRowDxfId="11" id="2" mc:Ignorable="xr xr3" name="Table2" ref="B3:H8" tableBorderDxfId="8" totalsRowBorderDxfId="7" totalsRowShown="0" xr:uid="{1D0FFA7F-7DA9-724C-B45B-9B3B656FBCA4}">
   <autoFilter ref="B3:H8" xr:uid="{1D0FFA7F-7DA9-724C-B45B-9B3B656FBCA4}"/>
   <tableColumns count="7">
-    <tableColumn dataDxfId="8" id="1" name="QueryTemplate" xr3:uid="{BCBFF39D-F8EE-FB4A-9663-295F85FEC319}"/>
-    <tableColumn dataDxfId="7" id="2" name="col1" xr3:uid="{36DE5603-B39C-B24E-A335-ADADF710349A}"/>
-    <tableColumn dataDxfId="6" id="3" name="col2" xr3:uid="{F667053C-0B9A-EE4E-94A6-058070DFA44F}"/>
-    <tableColumn dataDxfId="5" id="4" name="col3" xr3:uid="{A1B6C63C-A9AD-374E-BFC1-77E97FD26494}"/>
-    <tableColumn dataDxfId="4" id="5" name="col4" xr3:uid="{A626D9AC-E0DC-8C44-920B-C23E5E4A0422}"/>
-    <tableColumn dataDxfId="3" id="6" name="col5" xr3:uid="{EB858D0B-136A-3145-A25E-B2EDB9A06486}"/>
-    <tableColumn dataDxfId="2" id="7" name="col6" xr3:uid="{BC9C8CFC-3C12-DF49-9146-FAA384F36C04}"/>
+    <tableColumn dataDxfId="6" id="1" name="QueryTemplate" xr3:uid="{BCBFF39D-F8EE-FB4A-9663-295F85FEC319}"/>
+    <tableColumn dataDxfId="5" id="2" name="col1" xr3:uid="{36DE5603-B39C-B24E-A335-ADADF710349A}"/>
+    <tableColumn dataDxfId="4" id="3" name="col2" xr3:uid="{F667053C-0B9A-EE4E-94A6-058070DFA44F}"/>
+    <tableColumn dataDxfId="3" id="4" name="col3" xr3:uid="{A1B6C63C-A9AD-374E-BFC1-77E97FD26494}"/>
+    <tableColumn dataDxfId="2" id="5" name="col4" xr3:uid="{A626D9AC-E0DC-8C44-920B-C23E5E4A0422}"/>
+    <tableColumn dataDxfId="1" id="6" name="col5" xr3:uid="{EB858D0B-136A-3145-A25E-B2EDB9A06486}"/>
+    <tableColumn dataDxfId="0" id="7" name="col6" xr3:uid="{BC9C8CFC-3C12-DF49-9146-FAA384F36C04}"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -981,7 +981,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme 2013 - 2022" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -991,7 +991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2395513-0369-7445-AF2F-A248C4C2C245}">
   <dimension ref="B3:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -1203,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D4405E-6490-7540-8653-977CD177E976}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>